<commit_message>
xog excel sv chưa có nơi tt  kết quả sv
</commit_message>
<xml_diff>
--- a/admin/exel/product_import.xlsx
+++ b/admin/exel/product_import.xlsx
@@ -355,10 +355,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -377,20 +377,6 @@
       <c r="D2"/>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>